<commit_message>
Added End to End Examdesk flow | Dashboard Ongoing Test Automation Test Cases | All Types of Question Addition
</commit_message>
<xml_diff>
--- a/Automation/src/main/resources/configfile/TestData.xlsx
+++ b/Automation/src/main/resources/configfile/TestData.xlsx
@@ -5,14 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proctur Admin\Desktop\Automation framework\Automation\src\main\resources\configfile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\clone\ExamdeskAuto\Automation\src\main\resources\configfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12870" windowHeight="5070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12870" windowHeight="5070" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="singleChoice" sheetId="1" r:id="rId1"/>
+    <sheet name="multipleChoice" sheetId="2" r:id="rId2"/>
+    <sheet name="matchMatrix" sheetId="4" r:id="rId3"/>
+    <sheet name="true" sheetId="6" r:id="rId4"/>
+    <sheet name="matchTheFollowing" sheetId="7" r:id="rId5"/>
+    <sheet name="autoSubjectivetype" sheetId="8" r:id="rId6"/>
+    <sheet name="manualSubjectiveType" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,41 +30,154 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="9">
-  <si>
-    <t>TestName</t>
-  </si>
-  <si>
-    <t>TestSteps</t>
-  </si>
-  <si>
-    <t>TestComments</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login </t>
-  </si>
-  <si>
-    <t>LoginSteps</t>
-  </si>
-  <si>
-    <t>LoginComments</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>kmm1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+  <si>
+    <t>option1</t>
+  </si>
+  <si>
+    <t>option2</t>
+  </si>
+  <si>
+    <t>option3</t>
+  </si>
+  <si>
+    <t>option4</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>this is single choice question added?</t>
+  </si>
+  <si>
+    <t>given option1</t>
+  </si>
+  <si>
+    <t>given option2</t>
+  </si>
+  <si>
+    <t>given option3</t>
+  </si>
+  <si>
+    <t>given option4</t>
+  </si>
+  <si>
+    <t>dsomocwsc l</t>
+  </si>
+  <si>
+    <t>startQuestion</t>
+  </si>
+  <si>
+    <t>this is Multiple choice question added?</t>
+  </si>
+  <si>
+    <t>MC option1</t>
+  </si>
+  <si>
+    <t>MC given option2</t>
+  </si>
+  <si>
+    <t>MC given option3</t>
+  </si>
+  <si>
+    <t>MC given option4</t>
+  </si>
+  <si>
+    <t>Multiple Choice</t>
+  </si>
+  <si>
+    <t>option5</t>
+  </si>
+  <si>
+    <t>option6</t>
+  </si>
+  <si>
+    <t>option7</t>
+  </si>
+  <si>
+    <t>option8</t>
+  </si>
+  <si>
+    <t>MM option1</t>
+  </si>
+  <si>
+    <t>MM given option2</t>
+  </si>
+  <si>
+    <t>MF option1</t>
+  </si>
+  <si>
+    <t>MF given option2</t>
+  </si>
+  <si>
+    <t>MF given option3</t>
+  </si>
+  <si>
+    <t>MF given option4</t>
+  </si>
+  <si>
+    <t>this is Match Matrix question added?</t>
+  </si>
+  <si>
+    <t>MM given option3</t>
+  </si>
+  <si>
+    <t>MM given option4</t>
+  </si>
+  <si>
+    <t>MM   option1</t>
+  </si>
+  <si>
+    <t>MM  given option3</t>
+  </si>
+  <si>
+    <t>Match matrix question</t>
+  </si>
+  <si>
+    <t>this is true or false question added?</t>
+  </si>
+  <si>
+    <t>true or false  question</t>
+  </si>
+  <si>
+    <t>this is Match following question added?</t>
+  </si>
+  <si>
+    <t>MF  option1</t>
+  </si>
+  <si>
+    <t>MF  given option3</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>what is subjective type auto evaluation?</t>
+  </si>
+  <si>
+    <t>what is subjective type manual evaluation question?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -86,8 +205,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,120 +488,415 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>